<commit_message>
Ejercicio de distancia euclidiana
</commit_message>
<xml_diff>
--- a/19_Top_selec_de_tecnologia_de_infor/Ejercicio 1.xlsx
+++ b/19_Top_selec_de_tecnologia_de_infor/Ejercicio 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\9 semestre\19_Top_selec_de_tecnologia_de_infor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D41C6DD-EC8B-44D8-BB16-785D5B28ED6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2845B34E-A66B-4560-9325-1F3EE386E3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF15050D-5EFB-49D1-AE47-C846F6D85A7D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Banda</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Suma y raiz</t>
+  </si>
+  <si>
+    <t>Deacuerdo a la relacion entre Gregorio y Perla, Para gregorio los valores faltantes serian 1(Guns n roses), 3(Pink Floyd) y 3(The rolling) respectivamente</t>
   </si>
 </sst>
 </file>
@@ -115,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +218,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF33CC33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -265,7 +274,8 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -274,14 +284,14 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CC33"/>
+      <color rgb="FF009900"/>
+      <color rgb="FFFF3300"/>
       <color rgb="FFFFCCFF"/>
-      <color rgb="FF009900"/>
-      <color rgb="FF33CC33"/>
       <color rgb="FF66FF33"/>
       <color rgb="FFFF9966"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFFF9933"/>
-      <color rgb="FFFF3300"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FFFFFFCC"/>
     </mruColors>
@@ -295,54 +305,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>41413</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>30763</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>68628</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>162590</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BBFDFD6-FA81-EB0F-7553-E57049A7C036}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="1853" t="24812" r="5950" b="46150"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="41413" y="2316763"/>
-          <a:ext cx="13006063" cy="2227327"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -642,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01AED3CB-887A-4B27-8536-F6040727690C}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,31 +690,31 @@
         <v>4</v>
       </c>
       <c r="K2" s="10">
-        <f>(IF(AND($B2&gt;0,C2&gt;0),$B2-C2,0))^2</f>
+        <f t="shared" ref="K2:Q2" si="0">(IF(AND($B2&gt;0,C2&gt;0),$B2-C2,0))^2</f>
         <v>6.25</v>
       </c>
       <c r="L2" s="9">
-        <f>(IF(AND($B2&gt;0,D2&gt;0),$B2-D2,0))^2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="M2" s="8">
-        <f>(IF(AND($B2&gt;0,E2&gt;0),$B2-E2,0))^2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="N2" s="7">
-        <f>(IF(AND($B2&gt;0,F2&gt;0),$B2-F2,0))^2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O2" s="6">
-        <f>(IF(AND($B2&gt;0,G2&gt;0),$B2-G2,0))^2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P2" s="5">
-        <f>(IF(AND($B2&gt;0,H2&gt;0),$B2-H2,0))^2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="Q2" s="4">
-        <f>(IF(AND($B2&gt;0,I2&gt;0),$B2-I2,0))^2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -783,31 +745,31 @@
       </c>
       <c r="I3" s="4"/>
       <c r="K3" s="10">
-        <f t="shared" ref="K3:K9" si="0">(IF(AND($B3&gt;0,C3&gt;0),$B3-C3,0))^2</f>
+        <f t="shared" ref="K3:K9" si="1">(IF(AND($B3&gt;0,C3&gt;0),$B3-C3,0))^2</f>
         <v>1</v>
       </c>
       <c r="L3" s="9">
-        <f t="shared" ref="L3:L9" si="1">(IF(AND($B3&gt;0,D3&gt;0),$B3-D3,0))^2</f>
+        <f t="shared" ref="L3:L9" si="2">(IF(AND($B3&gt;0,D3&gt;0),$B3-D3,0))^2</f>
         <v>6.25</v>
       </c>
       <c r="M3" s="8">
-        <f t="shared" ref="M3:M9" si="2">(IF(AND($B3&gt;0,E3&gt;0),$B3-E3,0))^2</f>
+        <f t="shared" ref="M3:M9" si="3">(IF(AND($B3&gt;0,E3&gt;0),$B3-E3,0))^2</f>
         <v>9</v>
       </c>
       <c r="N3" s="7">
-        <f t="shared" ref="N3:N9" si="3">(IF(AND($B3&gt;0,F3&gt;0),$B3-F3,0))^2</f>
+        <f t="shared" ref="N3:N9" si="4">(IF(AND($B3&gt;0,F3&gt;0),$B3-F3,0))^2</f>
         <v>4</v>
       </c>
       <c r="O3" s="6">
-        <f t="shared" ref="O3:O9" si="4">(IF(AND($B3&gt;0,G3&gt;0),$B3-G3,0))^2</f>
+        <f t="shared" ref="O3:O9" si="5">(IF(AND($B3&gt;0,G3&gt;0),$B3-G3,0))^2</f>
         <v>2.25</v>
       </c>
       <c r="P3" s="5">
-        <f t="shared" ref="P3:P9" si="5">(IF(AND($B3&gt;0,H3&gt;0),$B3-H3,0))^2</f>
+        <f t="shared" ref="P3:P9" si="6">(IF(AND($B3&gt;0,H3&gt;0),$B3-H3,0))^2</f>
         <v>16</v>
       </c>
       <c r="Q3" s="4">
-        <f t="shared" ref="Q3:Q9" si="6">(IF(AND($B3&gt;0,I3&gt;0),$B3-I3,0))^2</f>
+        <f t="shared" ref="Q3:Q9" si="7">(IF(AND($B3&gt;0,I3&gt;0),$B3-I3,0))^2</f>
         <v>0</v>
       </c>
     </row>
@@ -834,31 +796,31 @@
         <v>1</v>
       </c>
       <c r="K4" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L4" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N4" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O4" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P4" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -881,31 +843,31 @@
         <v>5</v>
       </c>
       <c r="K5" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L5" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N5" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O5" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P5" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -936,31 +898,31 @@
       </c>
       <c r="I6" s="4"/>
       <c r="K6" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="L6" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N6" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O6" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P6" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -987,31 +949,31 @@
       </c>
       <c r="I7" s="4"/>
       <c r="K7" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="L7" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="M7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.25</v>
       </c>
       <c r="N7" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O7" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P7" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.25</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1038,31 +1000,31 @@
         <v>3</v>
       </c>
       <c r="K8" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N8" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P8" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1091,31 +1053,31 @@
         <v>3</v>
       </c>
       <c r="K9" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L9" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N9" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O9" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P9" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1124,245 +1086,51 @@
         <v>24</v>
       </c>
       <c r="K10" s="15">
-        <f>SQRT(SUM(K2:K9))</f>
-        <v>3.3911649915626341</v>
+        <f>ROUND(SQRT(SUM(K2:K9)),2)</f>
+        <v>3.39</v>
       </c>
       <c r="L10" s="14">
-        <f t="shared" ref="L10:Q10" si="7">SQRT(SUM(L2:L9))</f>
+        <f>ROUND(SQRT(SUM(L2:L9)),2)</f>
         <v>3.5</v>
       </c>
       <c r="M10" s="13">
-        <f t="shared" si="7"/>
-        <v>5.024937810560445</v>
+        <f>ROUND(SQRT(SUM(M2:M9)),2)</f>
+        <v>5.0199999999999996</v>
       </c>
       <c r="N10" s="16">
-        <f t="shared" si="7"/>
+        <f>ROUND(SQRT(SUM(N2:N9)),2)</f>
         <v>2</v>
       </c>
-      <c r="O10" s="17">
-        <f t="shared" si="7"/>
-        <v>2.0615528128088303</v>
+      <c r="O10" s="11">
+        <f>ROUND(SQRT(SUM(O2:O9)),2)</f>
+        <v>2.06</v>
       </c>
       <c r="P10" s="12">
-        <f t="shared" si="7"/>
-        <v>5.2201532544552753</v>
-      </c>
-      <c r="Q10" s="11">
-        <f t="shared" si="7"/>
-        <v>1.4142135623730951</v>
+        <f>ROUND(SQRT(SUM(P2:P9)),2)</f>
+        <v>5.22</v>
+      </c>
+      <c r="Q10" s="17">
+        <f>ROUND(SQRT(SUM(Q2:Q9)),2)</f>
+        <v>1.41</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>